<commit_message>
12:32 time 07.04.2025 date
</commit_message>
<xml_diff>
--- a/file_service/qabul.xlsx
+++ b/file_service/qabul.xlsx
@@ -477,7 +477,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
@@ -656,6 +656,53 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Isokov Eldor Fayzullayevich</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Mehnat muhofazasi va texnika xavfsizligi</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>AD1460068</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>3140687256008</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Mirzo Ulugʻbek tumani</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>998971300087</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>

</xml_diff>

<commit_message>
15:48 time 17.04.2025 date
</commit_message>
<xml_diff>
--- a/file_service/qabul.xlsx
+++ b/file_service/qabul.xlsx
@@ -477,10 +477,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A4" sqref="A4:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -612,7 +612,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Amirov Akrom</t>
+          <t>Raxmatov islom Xusan o'g'li</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -622,7 +622,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Rus tili</t>
+          <t>O'zbek tili</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -632,74 +632,27 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>KA9874653</t>
+          <t>AD5538879</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>1234567890123</t>
+          <t>31408950420035</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Navoiy viloyati</t>
+          <t>Toshkent viloyati</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Uchquduq tumani</t>
+          <t>Olmaliq shahri</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>+12676860109</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Isokov Eldor Fayzullayevich</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Mehnat muhofazasi va texnika xavfsizligi</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>O'zbek tili</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Kunduzgi</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>AD1460068</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>3140687256008</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Toshkent shahri</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Mirzo Ulugʻbek tumani</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>998971300087</t>
+          <t>998931898188</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
12:28 time 19.04.2025 date
</commit_message>
<xml_diff>
--- a/file_service/qabul.xlsx
+++ b/file_service/qabul.xlsx
@@ -477,7 +477,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD7"/>
@@ -656,6 +656,194 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Oribjonov Islombek Xusniddin o'g'li</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Mehnat muhofazasi va texnika xavfsizligi</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Sirtqi</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>AD5879006</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>53006075130046</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Andijon viloyati</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Jalaquduq tuman</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>998335567538</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Ismoilov Alisher Adxamovich</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Menejment</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Sirtqi</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>AD0716061</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>51110056750049</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Yunusobod tumani</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>998337034905</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Miryaxyoyev Miralisher Mirxaydar o'g'li</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Metrologiya va standartlashtirish</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Sirtqi</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>AD7947777</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>30605986780015</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Toshkent viloyati</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Qibray tumani</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>998937037330</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>/start</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Menejment</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Rus tili</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Sirtqi</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>AB6908896</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>51503016520051</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Shayxontohur tumani</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>998990677063</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>

</xml_diff>

<commit_message>
11:11 time 21.04.2025 date
</commit_message>
<xml_diff>
--- a/file_service/qabul.xlsx
+++ b/file_service/qabul.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pycharm\MIMA_Bot\file_service\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A5DA78-9675-41D2-8E82-E9C7AA8AC245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DEBF801-7310-41CE-BD41-FA7C2D697359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="71">
   <si>
     <t>Mehnat va ijtimoiy munosabatlar akademiyasi 2025-2026 o'quv yiliga xujjat topshirgan abituryentlar ruyhati</t>
   </si>
@@ -49,40 +49,22 @@
     <t>Tuman</t>
   </si>
   <si>
+    <t>Telegram raqami</t>
+  </si>
+  <si>
     <t>Telefon raqami</t>
   </si>
   <si>
-    <t>Amirov Akrom</t>
-  </si>
-  <si>
-    <t>Bugalteriya hisobi</t>
+    <t>Sana</t>
+  </si>
+  <si>
+    <t>Raxmatov islom Xusan o'g'li</t>
+  </si>
+  <si>
+    <t>Mehnat muhofazasi va texnika xavfsizligi</t>
   </si>
   <si>
     <t>O'zbek tili</t>
-  </si>
-  <si>
-    <t>Kunduzgi</t>
-  </si>
-  <si>
-    <t>AB8098565</t>
-  </si>
-  <si>
-    <t>1234567890123</t>
-  </si>
-  <si>
-    <t>Xorazm viloyati</t>
-  </si>
-  <si>
-    <t>Urganch shahri</t>
-  </si>
-  <si>
-    <t>+12676860109</t>
-  </si>
-  <si>
-    <t>Raxmatov islom Xusan o'g'li</t>
-  </si>
-  <si>
-    <t>Mehnat muhofazasi va texnika xavfsizligi</t>
   </si>
   <si>
     <t>Sirtqi</t>
@@ -273,6 +255,7 @@
       <charset val="204"/>
     </font>
     <font>
+      <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -312,11 +295,11 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -324,12 +307,8 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -339,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -350,10 +329,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -635,23 +613,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="40.42578125" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" customWidth="1"/>
-    <col min="9" max="10" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" customWidth="1"/>
+    <col min="8" max="8" width="21.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -665,9 +645,9 @@
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
@@ -699,48 +679,54 @@
       <c r="I2" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="J2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
         <v>22</v>
@@ -763,51 +749,51 @@
         <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G6" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="H6" t="s">
         <v>38</v>
@@ -824,10 +810,10 @@
         <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E7" t="s">
         <v>42</v>
@@ -836,27 +822,27 @@
         <v>43</v>
       </c>
       <c r="G7" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="H7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E8" t="s">
         <v>48</v>
@@ -865,27 +851,27 @@
         <v>49</v>
       </c>
       <c r="G8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" t="s">
         <v>50</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>51</v>
-      </c>
-      <c r="I8" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" t="s">
         <v>53</v>
       </c>
-      <c r="B9" t="s">
-        <v>34</v>
-      </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E9" t="s">
         <v>54</v>
@@ -894,56 +880,56 @@
         <v>55</v>
       </c>
       <c r="G9" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="H9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G10" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E11" t="s">
         <v>67</v>
@@ -952,47 +938,18 @@
         <v>68</v>
       </c>
       <c r="G11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" t="s">
         <v>69</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>70</v>
-      </c>
-      <c r="I11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>72</v>
-      </c>
-      <c r="B12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" t="s">
-        <v>73</v>
-      </c>
-      <c r="F12" t="s">
-        <v>74</v>
-      </c>
-      <c r="G12" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" t="s">
-        <v>75</v>
-      </c>
-      <c r="I12" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
17:28 time 21.04.2025 date
</commit_message>
<xml_diff>
--- a/file_service/qabul.xlsx
+++ b/file_service/qabul.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pycharm\MIMA_Bot\file_service\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Asosiy\Proyekt\MIMA_Bot\file_service\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DEBF801-7310-41CE-BD41-FA7C2D697359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE643F2B-245E-47B7-A375-68C7D7F64221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="97">
   <si>
     <t>Mehnat va ijtimoiy munosabatlar akademiyasi 2025-2026 o'quv yiliga xujjat topshirgan abituryentlar ruyhati</t>
   </si>
@@ -85,6 +85,9 @@
     <t>998931898188</t>
   </si>
   <si>
+    <t>2025-04-12</t>
+  </si>
+  <si>
     <t>Oribjonov Islombek Xusniddin o'g'li</t>
   </si>
   <si>
@@ -103,6 +106,9 @@
     <t>998335567538</t>
   </si>
   <si>
+    <t>2025-04-13</t>
+  </si>
+  <si>
     <t>Ismoilov Alisher Adxamovich</t>
   </si>
   <si>
@@ -124,6 +130,9 @@
     <t>998337034905</t>
   </si>
   <si>
+    <t>2025-04-14</t>
+  </si>
+  <si>
     <t>Miryaxyoyev Miralisher Mirxaydar o'g'li</t>
   </si>
   <si>
@@ -142,6 +151,9 @@
     <t>998937037330</t>
   </si>
   <si>
+    <t>2025-04-15</t>
+  </si>
+  <si>
     <t>abdullayev muhammad ikrom ogli</t>
   </si>
   <si>
@@ -163,6 +175,9 @@
     <t>998972312424</t>
   </si>
   <si>
+    <t>2025-04-16</t>
+  </si>
+  <si>
     <t>Mahkamov Doniyor Baxtiyer o'g'li</t>
   </si>
   <si>
@@ -178,6 +193,9 @@
     <t>998933231850</t>
   </si>
   <si>
+    <t>2025-04-17</t>
+  </si>
+  <si>
     <t>Olimov O'ralbek Dilshod o'g'li</t>
   </si>
   <si>
@@ -199,6 +217,9 @@
     <t>998919862474</t>
   </si>
   <si>
+    <t>2025-04-18</t>
+  </si>
+  <si>
     <t>JALILOVA NOZIMA MUXIDDIN QIZI</t>
   </si>
   <si>
@@ -220,6 +241,9 @@
     <t>+998955259606</t>
   </si>
   <si>
+    <t>2025-04-19</t>
+  </si>
+  <si>
     <t>Tillaxodjayev Nurulloxon Axmadullayevich</t>
   </si>
   <si>
@@ -233,6 +257,60 @@
   </si>
   <si>
     <t>998902170505</t>
+  </si>
+  <si>
+    <t>2025-04-20</t>
+  </si>
+  <si>
+    <t>Eshmuratov Javohir Jahongir o'g'li</t>
+  </si>
+  <si>
+    <t>Kunduzgi</t>
+  </si>
+  <si>
+    <t>AD1587887</t>
+  </si>
+  <si>
+    <t>52605066240019</t>
+  </si>
+  <si>
+    <t>Surxondaryo viloyati</t>
+  </si>
+  <si>
+    <t>Termiz shahri</t>
+  </si>
+  <si>
+    <t>998975520026</t>
+  </si>
+  <si>
+    <t>+998975520026</t>
+  </si>
+  <si>
+    <t>2025-04-21</t>
+  </si>
+  <si>
+    <t>Chinpulotova Ruxsora Bekpulot qizi</t>
+  </si>
+  <si>
+    <t>Ijtimoiy ish</t>
+  </si>
+  <si>
+    <t>AE2391801</t>
+  </si>
+  <si>
+    <t>41211925360013</t>
+  </si>
+  <si>
+    <t>Buxoro viloyati</t>
+  </si>
+  <si>
+    <t>Shofirkon tumani</t>
+  </si>
+  <si>
+    <t>998935336133</t>
+  </si>
+  <si>
+    <t>+998941339133</t>
   </si>
 </sst>
 </file>
@@ -613,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,10 +792,16 @@
       <c r="I3" t="s">
         <v>20</v>
       </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
@@ -729,27 +813,33 @@
         <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I4" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="J4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
@@ -758,27 +848,33 @@
         <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I5" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="J5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
@@ -787,27 +883,33 @@
         <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F6" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G6" t="s">
         <v>18</v>
       </c>
       <c r="H6" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="I6" t="s">
-        <v>39</v>
+        <v>42</v>
+      </c>
+      <c r="J6" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
@@ -816,27 +918,33 @@
         <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F7" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G7" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="H7" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="I7" t="s">
-        <v>46</v>
+        <v>50</v>
+      </c>
+      <c r="J7" t="s">
+        <v>50</v>
+      </c>
+      <c r="K7" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
@@ -845,27 +953,33 @@
         <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="F8" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="G8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H8" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="I8" t="s">
-        <v>51</v>
+        <v>56</v>
+      </c>
+      <c r="J8" t="s">
+        <v>56</v>
+      </c>
+      <c r="K8" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
@@ -874,27 +988,33 @@
         <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F9" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="G9" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="H9" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="I9" t="s">
-        <v>58</v>
+        <v>64</v>
+      </c>
+      <c r="J9" t="s">
+        <v>64</v>
+      </c>
+      <c r="K9" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
@@ -903,27 +1023,33 @@
         <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="F10" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="G10" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="H10" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="I10" t="s">
-        <v>65</v>
+        <v>72</v>
+      </c>
+      <c r="J10" t="s">
+        <v>72</v>
+      </c>
+      <c r="K10" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
@@ -932,19 +1058,95 @@
         <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="F11" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="G11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H11" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="I11" t="s">
-        <v>70</v>
+        <v>78</v>
+      </c>
+      <c r="J11" t="s">
+        <v>78</v>
+      </c>
+      <c r="K11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" t="s">
+        <v>82</v>
+      </c>
+      <c r="F12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G12" t="s">
+        <v>84</v>
+      </c>
+      <c r="H12" t="s">
+        <v>85</v>
+      </c>
+      <c r="I12" t="s">
+        <v>86</v>
+      </c>
+      <c r="J12" t="s">
+        <v>87</v>
+      </c>
+      <c r="K12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s">
+        <v>91</v>
+      </c>
+      <c r="F13" t="s">
+        <v>92</v>
+      </c>
+      <c r="G13" t="s">
+        <v>93</v>
+      </c>
+      <c r="H13" t="s">
+        <v>94</v>
+      </c>
+      <c r="I13" t="s">
+        <v>95</v>
+      </c>
+      <c r="J13" t="s">
+        <v>96</v>
+      </c>
+      <c r="K13" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
17:13 time 25.04.2025 date
</commit_message>
<xml_diff>
--- a/file_service/qabul.xlsx
+++ b/file_service/qabul.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A14" sqref="A14:XFD14"/>
@@ -1462,6 +1462,63 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Aydinova Narine Sergeevna</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Rus tili</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>AD6055389</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>60402085220078</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Mirzo Ulugʻbek tumani</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>998909340132</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>+998935617938</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>2025-04-25</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:K1"/>

</xml_diff>

<commit_message>
9:28 time 28.04.2025 date
</commit_message>
<xml_diff>
--- a/file_service/qabul.xlsx
+++ b/file_service/qabul.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A14" sqref="A14:XFD14"/>
@@ -1519,6 +1519,120 @@
         </is>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Xudoyorov Muslimjon Mominjon ogli</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Sirtqi</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>AD7761080</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>31103914340034</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Margʻilon tumani</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>998901669999</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>+998916588000</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>2025-04-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Adizov Ismoiljon</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Sirtqi</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>AD4325461</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>32804881070096</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Mirzo Ulugʻbek tumani</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>998903490733</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>+998936578677</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>2025-04-27</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:K1"/>

</xml_diff>

<commit_message>
10:17 time 28.04.2025 date
</commit_message>
<xml_diff>
--- a/file_service/qabul.xlsx
+++ b/file_service/qabul.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Asosiy\PyCharm\MIMA_Bot\file_service\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32118DD6-F4F7-47B7-B4B0-4191BC65FFDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85E6EFF-C7CD-47E1-AB28-FE365400651E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="150">
   <si>
     <t>Mehnat va ijtimoiy munosabatlar akademiyasi 2025-2026 o'quv yiliga xujjat topshirgan abituryentlar ruyhati</t>
   </si>
@@ -413,6 +413,63 @@
   </si>
   <si>
     <t>2025-04-24</t>
+  </si>
+  <si>
+    <t>Aydinova Narine Sergeevna</t>
+  </si>
+  <si>
+    <t>Rus tili</t>
+  </si>
+  <si>
+    <t>AD6055389</t>
+  </si>
+  <si>
+    <t>60402085220078</t>
+  </si>
+  <si>
+    <t>998909340132</t>
+  </si>
+  <si>
+    <t>+998935617938</t>
+  </si>
+  <si>
+    <t>2025-04-25</t>
+  </si>
+  <si>
+    <t>Xudoyorov Muslimjon Mominjon ogli</t>
+  </si>
+  <si>
+    <t>AD7761080</t>
+  </si>
+  <si>
+    <t>31103914340034</t>
+  </si>
+  <si>
+    <t>Margʻilon tumani</t>
+  </si>
+  <si>
+    <t>998901669999</t>
+  </si>
+  <si>
+    <t>+998916588000</t>
+  </si>
+  <si>
+    <t>2025-04-27</t>
+  </si>
+  <si>
+    <t>Adizov Ismoiljon</t>
+  </si>
+  <si>
+    <t>AD4325461</t>
+  </si>
+  <si>
+    <t>32804881070096</t>
+  </si>
+  <si>
+    <t>998903490733</t>
+  </si>
+  <si>
+    <t>+998936578677</t>
   </si>
 </sst>
 </file>
@@ -793,10 +850,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+      <selection activeCell="A19" sqref="A19:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1426,7 +1483,111 @@
         <v>130</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>131</v>
+      </c>
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D19" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19" t="s">
+        <v>133</v>
+      </c>
+      <c r="F19" t="s">
+        <v>134</v>
+      </c>
+      <c r="G19" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19" t="s">
+        <v>55</v>
+      </c>
+      <c r="I19" t="s">
+        <v>135</v>
+      </c>
+      <c r="J19" t="s">
+        <v>136</v>
+      </c>
+      <c r="K19" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>138</v>
+      </c>
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" t="s">
+        <v>139</v>
+      </c>
+      <c r="F20" t="s">
+        <v>140</v>
+      </c>
+      <c r="G20" t="s">
+        <v>114</v>
+      </c>
+      <c r="H20" t="s">
+        <v>141</v>
+      </c>
+      <c r="I20" t="s">
+        <v>142</v>
+      </c>
+      <c r="J20" t="s">
+        <v>143</v>
+      </c>
+      <c r="K20" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>145</v>
+      </c>
+      <c r="B21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" t="s">
+        <v>146</v>
+      </c>
+      <c r="F21" t="s">
+        <v>147</v>
+      </c>
+      <c r="G21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H21" t="s">
+        <v>55</v>
+      </c>
+      <c r="I21" t="s">
+        <v>148</v>
+      </c>
+      <c r="J21" t="s">
+        <v>149</v>
+      </c>
+      <c r="K21" t="s">
+        <v>144</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:K1"/>

</xml_diff>

<commit_message>
10:28 time 30.04.2025 date
</commit_message>
<xml_diff>
--- a/file_service/qabul.xlsx
+++ b/file_service/qabul.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Asosiy\PyCharm\MIMA_Bot\file_service\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Asosiy\Proyekt\MIMA_Bot\file_service\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85E6EFF-C7CD-47E1-AB28-FE365400651E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BBCD05-F216-435A-AF92-1401DDCBA7ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="149">
   <si>
     <t>Mehnat va ijtimoiy munosabatlar akademiyasi 2025-2026 o'quv yiliga xujjat topshirgan abituryentlar ruyhati</t>
   </si>
@@ -101,9 +101,6 @@
   </si>
   <si>
     <t>Jalaquduq tuman</t>
-  </si>
-  <si>
-    <t>998335567538</t>
   </si>
   <si>
     <t>2025-04-13</t>
@@ -555,7 +552,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -570,6 +567,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -853,7 +851,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD21"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,609 +981,609 @@
       <c r="H4" t="s">
         <v>26</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="6">
+        <v>998906222398</v>
+      </c>
+      <c r="J4" s="6">
+        <v>998906222398</v>
+      </c>
+      <c r="K4" t="s">
         <v>27</v>
-      </c>
-      <c r="J4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
         <v>29</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
         <v>30</v>
       </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>31</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>32</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>33</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>34</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" t="s">
         <v>35</v>
-      </c>
-      <c r="J5" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
         <v>37</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
         <v>38</v>
       </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>39</v>
-      </c>
-      <c r="F6" t="s">
-        <v>40</v>
       </c>
       <c r="G6" t="s">
         <v>18</v>
       </c>
       <c r="H6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" t="s">
         <v>41</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" t="s">
         <v>42</v>
-      </c>
-      <c r="J6" t="s">
-        <v>42</v>
-      </c>
-      <c r="K6" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
         <v>44</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
         <v>45</v>
       </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>46</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>47</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>48</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>49</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
+        <v>49</v>
+      </c>
+      <c r="K7" t="s">
         <v>50</v>
-      </c>
-      <c r="J7" t="s">
-        <v>50</v>
-      </c>
-      <c r="K7" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
         <v>52</v>
       </c>
-      <c r="B8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>53</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" t="s">
         <v>54</v>
       </c>
-      <c r="G8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>55</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
+        <v>55</v>
+      </c>
+      <c r="K8" t="s">
         <v>56</v>
-      </c>
-      <c r="J8" t="s">
-        <v>56</v>
-      </c>
-      <c r="K8" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" t="s">
         <v>58</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
         <v>59</v>
       </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>60</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>61</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>62</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>63</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
+        <v>63</v>
+      </c>
+      <c r="K9" t="s">
         <v>64</v>
-      </c>
-      <c r="J9" t="s">
-        <v>64</v>
-      </c>
-      <c r="K9" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" t="s">
         <v>66</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
         <v>67</v>
       </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>68</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>69</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>70</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>71</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
+        <v>71</v>
+      </c>
+      <c r="K10" t="s">
         <v>72</v>
-      </c>
-      <c r="J10" t="s">
-        <v>72</v>
-      </c>
-      <c r="K10" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
         <v>74</v>
       </c>
-      <c r="B11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>75</v>
-      </c>
-      <c r="F11" t="s">
-        <v>76</v>
       </c>
       <c r="G11" t="s">
         <v>25</v>
       </c>
       <c r="H11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I11" t="s">
         <v>77</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
+        <v>77</v>
+      </c>
+      <c r="K11" t="s">
         <v>78</v>
-      </c>
-      <c r="J11" t="s">
-        <v>78</v>
-      </c>
-      <c r="K11" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" t="s">
         <v>80</v>
       </c>
-      <c r="B12" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>81</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>82</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>83</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>84</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>85</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>86</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>87</v>
-      </c>
-      <c r="K12" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" t="s">
         <v>89</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s">
         <v>90</v>
       </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>91</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>92</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>93</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>94</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>95</v>
       </c>
-      <c r="J13" t="s">
-        <v>96</v>
-      </c>
       <c r="K13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
         <v>97</v>
       </c>
-      <c r="B14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>98</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>99</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>100</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>101</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>102</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>103</v>
-      </c>
-      <c r="K14" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" t="s">
         <v>105</v>
       </c>
-      <c r="B15" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>106</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
+        <v>61</v>
+      </c>
+      <c r="H15" t="s">
         <v>107</v>
       </c>
-      <c r="G15" t="s">
-        <v>62</v>
-      </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>108</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
+        <v>108</v>
+      </c>
+      <c r="K15" t="s">
         <v>109</v>
-      </c>
-      <c r="J15" t="s">
-        <v>109</v>
-      </c>
-      <c r="K15" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" t="s">
         <v>111</v>
       </c>
-      <c r="B16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>112</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>113</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>114</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>115</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>116</v>
       </c>
-      <c r="J16" t="s">
-        <v>117</v>
-      </c>
       <c r="K16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
         <v>118</v>
       </c>
-      <c r="B17" t="s">
-        <v>67</v>
-      </c>
-      <c r="C17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>119</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" t="s">
         <v>120</v>
       </c>
-      <c r="G17" t="s">
-        <v>33</v>
-      </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>121</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>122</v>
       </c>
-      <c r="J17" t="s">
-        <v>123</v>
-      </c>
       <c r="K17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>123</v>
+      </c>
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" t="s">
         <v>124</v>
       </c>
-      <c r="B18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>125</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" t="s">
         <v>126</v>
       </c>
-      <c r="G18" t="s">
-        <v>33</v>
-      </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>127</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>128</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>129</v>
-      </c>
-      <c r="K18" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>130</v>
+      </c>
+      <c r="B19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" t="s">
         <v>131</v>
       </c>
-      <c r="B19" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" t="s">
         <v>132</v>
       </c>
-      <c r="D19" t="s">
-        <v>81</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>133</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
+        <v>32</v>
+      </c>
+      <c r="H19" t="s">
+        <v>54</v>
+      </c>
+      <c r="I19" t="s">
         <v>134</v>
       </c>
-      <c r="G19" t="s">
-        <v>33</v>
-      </c>
-      <c r="H19" t="s">
-        <v>55</v>
-      </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>135</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K19" t="s">
         <v>136</v>
-      </c>
-      <c r="K19" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>137</v>
+      </c>
+      <c r="B20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" t="s">
         <v>138</v>
       </c>
-      <c r="B20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>139</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
+        <v>113</v>
+      </c>
+      <c r="H20" t="s">
         <v>140</v>
       </c>
-      <c r="G20" t="s">
-        <v>114</v>
-      </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>141</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>142</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>143</v>
-      </c>
-      <c r="K20" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>144</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" t="s">
         <v>145</v>
       </c>
-      <c r="B21" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>146</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
+        <v>32</v>
+      </c>
+      <c r="H21" t="s">
+        <v>54</v>
+      </c>
+      <c r="I21" t="s">
         <v>147</v>
       </c>
-      <c r="G21" t="s">
-        <v>33</v>
-      </c>
-      <c r="H21" t="s">
-        <v>55</v>
-      </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>148</v>
       </c>
-      <c r="J21" t="s">
-        <v>149</v>
-      </c>
       <c r="K21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
12.05.2025 date 18:17 time
</commit_message>
<xml_diff>
--- a/file_service/qabul.xlsx
+++ b/file_service/qabul.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A22" sqref="A22:XFD22"/>
@@ -1747,6 +1747,63 @@
         </is>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Amirov Akrom</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>AA1234567</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>12345678901234</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Toshkent viloyati</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Olmaliq shahri</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>+998939849910</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>+998945289910</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>2025-05-07</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:K1"/>

</xml_diff>

<commit_message>
9:28 time 23.05.2025 date
</commit_message>
<xml_diff>
--- a/file_service/qabul.xlsx
+++ b/file_service/qabul.xlsx
@@ -454,7 +454,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M34"/>
+  <dimension ref="A1:M48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
@@ -2371,6 +2371,804 @@
         </is>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Raxmatov Ogabek</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>AD4419590</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>50908076150018</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Yashnaobod tumani</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>998336373784</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>+998931984133</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Boboqulova Bahora Sherzod qizi</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>AD6081128</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>60803066050143</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Ishtixon tumani</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>998944292086</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>+998944292086</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Malikova Shoxidaxon Zakirjanovna</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>AD7703787</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>41901891230031</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Andijon viloyati</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Andijon shahri</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>998999767752</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>+998999767752</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>2025-05-13</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Qudratov Sarvar Raximjon ogli</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>AD3368539</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>50604075670019</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Olmazor tumani</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>998940473807</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>+998330073407</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>2025-05-13</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>O'roqov Xushnudbek Xurshid o'g'li</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>AE2454790</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>51804076540053</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>Shayxontohur tumani</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>998999840771</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>+998999840771</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Iskandarov Sarvarbek Iskandar o'g'li</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>AD4799601</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>52911076170021</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>Kattaqoʻrgʻon tumani</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>998944475702</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>+998944475702</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Numonjonov Zuhriddin Abdulhafiz ogli</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>AD7653210</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>50612077080048</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>Margʻilon tumani</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>998911245111</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>+998331590053</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Muhammadaliyev Jahongir Mahmudjon ogli</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Psixologiya</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>AD5077856</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>50709066740028</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Toshkent viloyati</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>Yuqori Chirchiq tumani</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>998333515134</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>+998770174575</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Uaboyeva Sarvinoz Yusuf qizi</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>AD2635624</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>63011066300059</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Surxondaryo viloyati</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>Qumqoʻrgʻon tumani</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>998941727977</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>+998508890637</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>2025-05-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Xasan Saidmurodov</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>AD1999493</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>52305066180114</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>Payariq tumani</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>998957570177</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>+998997787117</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>2025-05-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Abdurxmon Tuychibayev Abdudjabbar o'g'li</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Bugalteriya hisobi</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>AD7006138</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>51409076620044</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>Yashnaobod tumani</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>998882802529</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>+998882802529</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>2025-05-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Rustamxojayev Javohirxoja muzaffarxon ogli</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>AD4246020</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>52001076610011</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>Olmazor tumani</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>998974432526</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>+998974432526</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Nabiyev Sirojiddin Farohiddin o'g'li</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>AD6788338</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>50102085150054</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Andijon viloyati</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>Asaka tumani</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>998507404744</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>+998914854913</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>MAMASALIEV SOBIR BAXTIYOROVICH</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Hayot faoliyati xavfsizligi</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Rus tili</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>AC2787580</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>52202047970013</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>Yashnaobod tumani</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>998944059922</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>+998880132242</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>2025-05-21</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:K1"/>

</xml_diff>

<commit_message>
9:34 time 25.06.2025 date
</commit_message>
<xml_diff>
--- a/file_service/qabul.xlsx
+++ b/file_service/qabul.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A22" sqref="A22:XFD22"/>
@@ -1804,6 +1804,120 @@
         </is>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>ATAMATOV ABDUXALIL SALAMOVICH</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Mehnat muhofazasi va texnika xavfsizligi</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>AB1234567</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>12345678901234</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Yakkasaroy tumani</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>+12676860109</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>+998945289910</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>2025-05-13</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>ATAMATOV ABDUXALIL SALAMOVICH</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Mehnat muhofazasi va texnika xavfsizligi</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>AB1234567</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>12345678901234</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Yakkasaroy tumani</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>+12676860109</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>+998945289910</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>2025-05-13</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:K1"/>

</xml_diff>

<commit_message>
1:49 time 26.06.2025 date
</commit_message>
<xml_diff>
--- a/file_service/qabul.xlsx
+++ b/file_service/qabul.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A22" sqref="A22:XFD22"/>
@@ -1918,6 +1918,63 @@
         </is>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Amirov Akrom Eshali ogli</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Hayot faoliyati xavfsizligi</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>AB5554414</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>12345678901234</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Xorazm viloyati</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Urganch shahri</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>+12676860109</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>+998945289910</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>2025-06-25</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:K1"/>

</xml_diff>

<commit_message>
20:25 time 28.06.2025 date
</commit_message>
<xml_diff>
--- a/file_service/qabul.xlsx
+++ b/file_service/qabul.xlsx
@@ -456,7 +456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M123"/>
+  <dimension ref="A1:M127"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
       <selection activeCell="E108" sqref="E108"/>
@@ -7448,6 +7448,234 @@
         </is>
       </c>
     </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>Murodullayev Asliddinjon Xurshidovich</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>AD4081875</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>51705075820037</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>Navoiy viloyati</t>
+        </is>
+      </c>
+      <c r="H124" t="inlineStr">
+        <is>
+          <t>Karmana tumani</t>
+        </is>
+      </c>
+      <c r="I124" t="inlineStr">
+        <is>
+          <t>998958222222</t>
+        </is>
+      </c>
+      <c r="J124" t="inlineStr">
+        <is>
+          <t>+998958222222</t>
+        </is>
+      </c>
+      <c r="K124" t="inlineStr">
+        <is>
+          <t>2025-06-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>Azizbek Isroilov Xusniddinovich</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>AD6928826</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>50201086580012</t>
+        </is>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H125" t="inlineStr">
+        <is>
+          <t>Uchtepa tumani</t>
+        </is>
+      </c>
+      <c r="I125" t="inlineStr">
+        <is>
+          <t>998909658251</t>
+        </is>
+      </c>
+      <c r="J125" t="inlineStr">
+        <is>
+          <t>+998909658251</t>
+        </is>
+      </c>
+      <c r="K125" t="inlineStr">
+        <is>
+          <t>2025-06-28</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>orifjonov dilshod</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>AD1569162</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>50509076920045</t>
+        </is>
+      </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="H126" t="inlineStr">
+        <is>
+          <t>Qo‘qon shahri</t>
+        </is>
+      </c>
+      <c r="I126" t="inlineStr">
+        <is>
+          <t>998911398039</t>
+        </is>
+      </c>
+      <c r="J126" t="inlineStr">
+        <is>
+          <t>+998911398039</t>
+        </is>
+      </c>
+      <c r="K126" t="inlineStr">
+        <is>
+          <t>2025-06-28</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>Xomidjonova Tamannoxon Axtamjon qizi</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>AD5616436</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>62305077010104</t>
+        </is>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="H127" t="inlineStr">
+        <is>
+          <t>Fargʻona tumani</t>
+        </is>
+      </c>
+      <c r="I127" t="inlineStr">
+        <is>
+          <t>998887602305</t>
+        </is>
+      </c>
+      <c r="J127" t="inlineStr">
+        <is>
+          <t>+998507142104</t>
+        </is>
+      </c>
+      <c r="K127" t="inlineStr">
+        <is>
+          <t>2025-06-28</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="D1:D66"/>
   <mergeCells count="1">

</xml_diff>

<commit_message>
12:20 time 01.07.2025 date
</commit_message>
<xml_diff>
--- a/file_service/qabul.xlsx
+++ b/file_service/qabul.xlsx
@@ -456,7 +456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M127"/>
+  <dimension ref="A1:M140"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
       <selection activeCell="E108" sqref="E108"/>
@@ -7676,6 +7676,747 @@
         </is>
       </c>
     </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>FARMONOVA ZARINA</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>Psixologiya</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>AD5184165</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>60109076960015</t>
+        </is>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H128" t="inlineStr">
+        <is>
+          <t>Yashnaobod tumani</t>
+        </is>
+      </c>
+      <c r="I128" t="inlineStr">
+        <is>
+          <t>998911623523</t>
+        </is>
+      </c>
+      <c r="J128" t="inlineStr">
+        <is>
+          <t>+998918102334</t>
+        </is>
+      </c>
+      <c r="K128" t="inlineStr">
+        <is>
+          <t>2025-06-29</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>Eshmuratov Jaloliddin Tohir o'g'li</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>AD0610768</t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>50909045470038</t>
+        </is>
+      </c>
+      <c r="G129" t="inlineStr">
+        <is>
+          <t>Jizzax viloyati</t>
+        </is>
+      </c>
+      <c r="H129" t="inlineStr">
+        <is>
+          <t>Zomin tumani</t>
+        </is>
+      </c>
+      <c r="I129" t="inlineStr">
+        <is>
+          <t>998949474230</t>
+        </is>
+      </c>
+      <c r="J129" t="inlineStr">
+        <is>
+          <t>+998957600076</t>
+        </is>
+      </c>
+      <c r="K129" t="inlineStr">
+        <is>
+          <t>2025-06-29</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>Halilov Abdurauf</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>Rus tili</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>AD3879501</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>32703922200035</t>
+        </is>
+      </c>
+      <c r="G130" t="inlineStr">
+        <is>
+          <t>Toshkent viloyati</t>
+        </is>
+      </c>
+      <c r="H130" t="inlineStr">
+        <is>
+          <t>Angren shahri</t>
+        </is>
+      </c>
+      <c r="I130" t="inlineStr">
+        <is>
+          <t>998937355565</t>
+        </is>
+      </c>
+      <c r="J130" t="inlineStr">
+        <is>
+          <t>+998937355565</t>
+        </is>
+      </c>
+      <c r="K130" t="inlineStr">
+        <is>
+          <t>2025-06-29</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>Oktamova ruhshona</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>AD6121348</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>60810067170055</t>
+        </is>
+      </c>
+      <c r="G131" t="inlineStr">
+        <is>
+          <t>Xorazm viloyati</t>
+        </is>
+      </c>
+      <c r="H131" t="inlineStr">
+        <is>
+          <t>Shovot tumani</t>
+        </is>
+      </c>
+      <c r="I131" t="inlineStr">
+        <is>
+          <t>998939140812</t>
+        </is>
+      </c>
+      <c r="J131" t="inlineStr">
+        <is>
+          <t>+998943106633</t>
+        </is>
+      </c>
+      <c r="K131" t="inlineStr">
+        <is>
+          <t>2025-06-29</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>Bu qaysi harf</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>AD2755823</t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>32904931690024</t>
+        </is>
+      </c>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>Jizzax viloyati</t>
+        </is>
+      </c>
+      <c r="H132" t="inlineStr">
+        <is>
+          <t>Yangiobod tumani</t>
+        </is>
+      </c>
+      <c r="I132" t="inlineStr">
+        <is>
+          <t>998955779302</t>
+        </is>
+      </c>
+      <c r="J132" t="inlineStr">
+        <is>
+          <t>+998955779302</t>
+        </is>
+      </c>
+      <c r="K132" t="inlineStr">
+        <is>
+          <t>2025-06-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>Kim Yuriy</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>Mehnat muhofazasi va texnika xavfsizligi</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>Rus tili</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>AD3569381</t>
+        </is>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>32008781930014</t>
+        </is>
+      </c>
+      <c r="G133" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H133" t="inlineStr">
+        <is>
+          <t>Mirzo Ulugʻbek tumani</t>
+        </is>
+      </c>
+      <c r="I133" t="inlineStr">
+        <is>
+          <t>+998977337388</t>
+        </is>
+      </c>
+      <c r="J133" t="inlineStr">
+        <is>
+          <t>+998977337388</t>
+        </is>
+      </c>
+      <c r="K133" t="inlineStr">
+        <is>
+          <t>2025-06-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>Boratov Vohidjon Erkinboy o'g'li</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>AD4095733</t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>30302924280027</t>
+        </is>
+      </c>
+      <c r="G134" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="H134" t="inlineStr">
+        <is>
+          <t>Dangʻara tumani</t>
+        </is>
+      </c>
+      <c r="I134" t="inlineStr">
+        <is>
+          <t>+998905868787</t>
+        </is>
+      </c>
+      <c r="J134" t="inlineStr">
+        <is>
+          <t>+998500117747</t>
+        </is>
+      </c>
+      <c r="K134" t="inlineStr">
+        <is>
+          <t>2025-06-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>Rajabova Iroda Obid qizi</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>AD3282682</t>
+        </is>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>62608076060115</t>
+        </is>
+      </c>
+      <c r="G135" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="H135" t="inlineStr">
+        <is>
+          <t>Kattaqoʻrgʻon tumani</t>
+        </is>
+      </c>
+      <c r="I135" t="inlineStr">
+        <is>
+          <t>998940149199</t>
+        </is>
+      </c>
+      <c r="J135" t="inlineStr">
+        <is>
+          <t>+998947535885</t>
+        </is>
+      </c>
+      <c r="K135" t="inlineStr">
+        <is>
+          <t>2025-06-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>Nishonva Dildora Ziyodulla qizi</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>AC2650600</t>
+        </is>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>41606956420012</t>
+        </is>
+      </c>
+      <c r="G136" t="inlineStr">
+        <is>
+          <t>Sirdaryo viloyati</t>
+        </is>
+      </c>
+      <c r="H136" t="inlineStr">
+        <is>
+          <t>Sardoba tumani</t>
+        </is>
+      </c>
+      <c r="I136" t="inlineStr">
+        <is>
+          <t>998979061122</t>
+        </is>
+      </c>
+      <c r="J136" t="inlineStr">
+        <is>
+          <t>+998979061122</t>
+        </is>
+      </c>
+      <c r="K136" t="inlineStr">
+        <is>
+          <t>2025-06-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>Toshpulatov Jamshid Xodjiakbar o'g'li</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>Rus tili</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>AD3351907</t>
+        </is>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>31104920270760</t>
+        </is>
+      </c>
+      <c r="G137" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H137" t="inlineStr">
+        <is>
+          <t>Yashnaobod tumani</t>
+        </is>
+      </c>
+      <c r="I137" t="inlineStr">
+        <is>
+          <t>998935477271</t>
+        </is>
+      </c>
+      <c r="J137" t="inlineStr">
+        <is>
+          <t>+998935477271</t>
+        </is>
+      </c>
+      <c r="K137" t="inlineStr">
+        <is>
+          <t>2025-06-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>Maqsudov Nurmuhammad shavkatjon ogli</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>AD6260332</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>51908065330644</t>
+        </is>
+      </c>
+      <c r="G138" t="inlineStr">
+        <is>
+          <t>Buxoro viloyati</t>
+        </is>
+      </c>
+      <c r="H138" t="inlineStr">
+        <is>
+          <t>Peshku tumani</t>
+        </is>
+      </c>
+      <c r="I138" t="inlineStr">
+        <is>
+          <t>998953540772</t>
+        </is>
+      </c>
+      <c r="J138" t="inlineStr">
+        <is>
+          <t>+998996846250</t>
+        </is>
+      </c>
+      <c r="K138" t="inlineStr">
+        <is>
+          <t>2025-06-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>Zakiryayeva Shirin Nurillayevna</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>Rus tili</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>AD1874714</t>
+        </is>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>41310826180015</t>
+        </is>
+      </c>
+      <c r="G139" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="H139" t="inlineStr">
+        <is>
+          <t>Samarqand shahri</t>
+        </is>
+      </c>
+      <c r="I139" t="inlineStr">
+        <is>
+          <t>998979244447</t>
+        </is>
+      </c>
+      <c r="J139" t="inlineStr">
+        <is>
+          <t>+998979244447</t>
+        </is>
+      </c>
+      <c r="K139" t="inlineStr">
+        <is>
+          <t>2025-07-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>Ochilova Ruxshona Abdurashidovna</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>AD3963854</t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>61403076150025</t>
+        </is>
+      </c>
+      <c r="G140" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="H140" t="inlineStr">
+        <is>
+          <t>Toyloq tumani</t>
+        </is>
+      </c>
+      <c r="I140" t="inlineStr">
+        <is>
+          <t>998507147607</t>
+        </is>
+      </c>
+      <c r="J140" t="inlineStr">
+        <is>
+          <t>+998507147607</t>
+        </is>
+      </c>
+      <c r="K140" t="inlineStr">
+        <is>
+          <t>2025-07-01</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="D1:D66"/>
   <mergeCells count="1">

</xml_diff>

<commit_message>
18:11 time 01.07.2025 date
</commit_message>
<xml_diff>
--- a/file_service/qabul.xlsx
+++ b/file_service/qabul.xlsx
@@ -456,7 +456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M140"/>
+  <dimension ref="A1:M145"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
       <selection activeCell="E108" sqref="E108"/>
@@ -8417,6 +8417,291 @@
         </is>
       </c>
     </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>Azamov Aziz</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>Hayot faoliyati xavfsizligi</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>AD5352798</t>
+        </is>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>52810076230020</t>
+        </is>
+      </c>
+      <c r="G141" t="inlineStr">
+        <is>
+          <t>Surxondaryo viloyati</t>
+        </is>
+      </c>
+      <c r="H141" t="inlineStr">
+        <is>
+          <t>Denov tumani</t>
+        </is>
+      </c>
+      <c r="I141" t="inlineStr">
+        <is>
+          <t>998938239646</t>
+        </is>
+      </c>
+      <c r="J141" t="inlineStr">
+        <is>
+          <t>+998938239646</t>
+        </is>
+      </c>
+      <c r="K141" t="inlineStr">
+        <is>
+          <t>2025-07-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>XASANOVA SEVINCHXON AXRORBEK QIZI</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>Rus tili</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>AC2540058</t>
+        </is>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>60810036940010</t>
+        </is>
+      </c>
+      <c r="G142" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H142" t="inlineStr">
+        <is>
+          <t>Yangihayot tumani</t>
+        </is>
+      </c>
+      <c r="I142" t="inlineStr">
+        <is>
+          <t>998944941008</t>
+        </is>
+      </c>
+      <c r="J142" t="inlineStr">
+        <is>
+          <t>+998944941008</t>
+        </is>
+      </c>
+      <c r="K142" t="inlineStr">
+        <is>
+          <t>2025-07-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>Sayfiddinova Maqsad Sherzodovna</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>AD5715114</t>
+        </is>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>60910076150056</t>
+        </is>
+      </c>
+      <c r="G143" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="H143" t="inlineStr">
+        <is>
+          <t>Toyloq tumani</t>
+        </is>
+      </c>
+      <c r="I143" t="inlineStr">
+        <is>
+          <t>998948370910</t>
+        </is>
+      </c>
+      <c r="J143" t="inlineStr">
+        <is>
+          <t>+998993507867</t>
+        </is>
+      </c>
+      <c r="K143" t="inlineStr">
+        <is>
+          <t>2025-07-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>Bekmurodov Sardor Shuhratovich</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>AD9500428</t>
+        </is>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>51608076270020</t>
+        </is>
+      </c>
+      <c r="G144" t="inlineStr">
+        <is>
+          <t>Surxondaryo viloyati</t>
+        </is>
+      </c>
+      <c r="H144" t="inlineStr">
+        <is>
+          <t>Termiz shahri</t>
+        </is>
+      </c>
+      <c r="I144" t="inlineStr">
+        <is>
+          <t>998996212007</t>
+        </is>
+      </c>
+      <c r="J144" t="inlineStr">
+        <is>
+          <t>+998942003007</t>
+        </is>
+      </c>
+      <c r="K144" t="inlineStr">
+        <is>
+          <t>2025-07-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>Po'latov Fayzulloh Kamoliddin o'g'li</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>Menejment</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>AD8066834</t>
+        </is>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>51607086540127</t>
+        </is>
+      </c>
+      <c r="G145" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H145" t="inlineStr">
+        <is>
+          <t>Shayxontohur tumani</t>
+        </is>
+      </c>
+      <c r="I145" t="inlineStr">
+        <is>
+          <t>998994778754</t>
+        </is>
+      </c>
+      <c r="J145" t="inlineStr">
+        <is>
+          <t>+998949928754</t>
+        </is>
+      </c>
+      <c r="K145" t="inlineStr">
+        <is>
+          <t>2025-07-01</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="D1:D66"/>
   <mergeCells count="1">

</xml_diff>

<commit_message>
10:02 time 02.07.2025 date
</commit_message>
<xml_diff>
--- a/file_service/qabul.xlsx
+++ b/file_service/qabul.xlsx
@@ -456,10 +456,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M145"/>
+  <dimension ref="A1:M151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="E108" sqref="E108"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="A132" sqref="A132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -7907,7 +7907,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Bu qaysi harf</t>
+          <t>IRSALIYEV TO‘YCHIBOY OTAKUZI O‘G‘LI</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -8699,6 +8699,348 @@
       <c r="K145" t="inlineStr">
         <is>
           <t>2025-07-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>Sa'dinov Husen Islomovich</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>AD1956155</t>
+        </is>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>52005056150012</t>
+        </is>
+      </c>
+      <c r="G146" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="H146" t="inlineStr">
+        <is>
+          <t>Toyloq tumani</t>
+        </is>
+      </c>
+      <c r="I146" t="inlineStr">
+        <is>
+          <t>998992949844</t>
+        </is>
+      </c>
+      <c r="J146" t="inlineStr">
+        <is>
+          <t>+998990488733</t>
+        </is>
+      </c>
+      <c r="K146" t="inlineStr">
+        <is>
+          <t>2025-07-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>Begmatov Hojiakbar Ulugbek ogli</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>AD7482039</t>
+        </is>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>51912076580039</t>
+        </is>
+      </c>
+      <c r="G147" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H147" t="inlineStr">
+        <is>
+          <t>Yashnaobod tumani</t>
+        </is>
+      </c>
+      <c r="I147" t="inlineStr">
+        <is>
+          <t>998906610323</t>
+        </is>
+      </c>
+      <c r="J147" t="inlineStr">
+        <is>
+          <t>+998906610323</t>
+        </is>
+      </c>
+      <c r="K147" t="inlineStr">
+        <is>
+          <t>2025-07-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>Xushboqov Bunyod Toxirovich</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>AD6046888</t>
+        </is>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>51202076350025</t>
+        </is>
+      </c>
+      <c r="G148" t="inlineStr">
+        <is>
+          <t>Surxondaryo viloyati</t>
+        </is>
+      </c>
+      <c r="H148" t="inlineStr">
+        <is>
+          <t>Termiz shahri</t>
+        </is>
+      </c>
+      <c r="I148" t="inlineStr">
+        <is>
+          <t>998994261253</t>
+        </is>
+      </c>
+      <c r="J148" t="inlineStr">
+        <is>
+          <t>+998997161253</t>
+        </is>
+      </c>
+      <c r="K148" t="inlineStr">
+        <is>
+          <t>2025-07-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>Mavleeva Elsana Timurovna</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>Psixologiya</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>Rus tili</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>AD5687911</t>
+        </is>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>60301088660013</t>
+        </is>
+      </c>
+      <c r="G149" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H149" t="inlineStr">
+        <is>
+          <t>Yashnaobod tumani</t>
+        </is>
+      </c>
+      <c r="I149" t="inlineStr">
+        <is>
+          <t>998974321132</t>
+        </is>
+      </c>
+      <c r="J149" t="inlineStr">
+        <is>
+          <t>+998974321132</t>
+        </is>
+      </c>
+      <c r="K149" t="inlineStr">
+        <is>
+          <t>2025-07-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>Shokirova Dilafruz Eminjon qizi</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>Rus tili</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>AD3230069</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>61003076620056</t>
+        </is>
+      </c>
+      <c r="G150" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H150" t="inlineStr">
+        <is>
+          <t>Mirzo Ulugʻbek tumani</t>
+        </is>
+      </c>
+      <c r="I150" t="inlineStr">
+        <is>
+          <t>998900668474</t>
+        </is>
+      </c>
+      <c r="J150" t="inlineStr">
+        <is>
+          <t>+998331668474</t>
+        </is>
+      </c>
+      <c r="K150" t="inlineStr">
+        <is>
+          <t>2025-07-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>Tojiddinova Muzayyam</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>Rus tili</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>AD6092423</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>60702085140012</t>
+        </is>
+      </c>
+      <c r="G151" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H151" t="inlineStr">
+        <is>
+          <t>Yashnaobod tumani</t>
+        </is>
+      </c>
+      <c r="I151" t="inlineStr">
+        <is>
+          <t>998930639601</t>
+        </is>
+      </c>
+      <c r="J151" t="inlineStr">
+        <is>
+          <t>+998938390207</t>
+        </is>
+      </c>
+      <c r="K151" t="inlineStr">
+        <is>
+          <t>2025-07-02</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
16:38 time 02.07.2025 date
</commit_message>
<xml_diff>
--- a/file_service/qabul.xlsx
+++ b/file_service/qabul.xlsx
@@ -456,7 +456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M151"/>
+  <dimension ref="A1:M155"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
       <selection activeCell="A132" sqref="A132"/>
@@ -9044,6 +9044,234 @@
         </is>
       </c>
     </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>Fayzullayev Fatxullo</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>AE1624128</t>
+        </is>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>52008075500011</t>
+        </is>
+      </c>
+      <c r="G152" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H152" t="inlineStr">
+        <is>
+          <t>Yashnaobod tumani</t>
+        </is>
+      </c>
+      <c r="I152" t="inlineStr">
+        <is>
+          <t>998885223533</t>
+        </is>
+      </c>
+      <c r="J152" t="inlineStr">
+        <is>
+          <t>+998338390777</t>
+        </is>
+      </c>
+      <c r="K152" t="inlineStr">
+        <is>
+          <t>2025-07-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>Joraqulov Bahodir</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>AD6150839</t>
+        </is>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>50608075780064</t>
+        </is>
+      </c>
+      <c r="G153" t="inlineStr">
+        <is>
+          <t>Navoiy viloyati</t>
+        </is>
+      </c>
+      <c r="H153" t="inlineStr">
+        <is>
+          <t>Navbahor tumani</t>
+        </is>
+      </c>
+      <c r="I153" t="inlineStr">
+        <is>
+          <t>998774774313</t>
+        </is>
+      </c>
+      <c r="J153" t="inlineStr">
+        <is>
+          <t>+998774774313</t>
+        </is>
+      </c>
+      <c r="K153" t="inlineStr">
+        <is>
+          <t>2025-07-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>Berdiyev Jo'rabek</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>AB6139569</t>
+        </is>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>50107005800024</t>
+        </is>
+      </c>
+      <c r="G154" t="inlineStr">
+        <is>
+          <t>Jizzax viloyati</t>
+        </is>
+      </c>
+      <c r="H154" t="inlineStr">
+        <is>
+          <t>Sharof Rashidov tumani</t>
+        </is>
+      </c>
+      <c r="I154" t="inlineStr">
+        <is>
+          <t>998992428774</t>
+        </is>
+      </c>
+      <c r="J154" t="inlineStr">
+        <is>
+          <t>+998992428774</t>
+        </is>
+      </c>
+      <c r="K154" t="inlineStr">
+        <is>
+          <t>2025-07-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>Shorustamova Sabina Shoakbar qizi</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>Rus tili</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>AD5424978</t>
+        </is>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>62209076510013</t>
+        </is>
+      </c>
+      <c r="G155" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H155" t="inlineStr">
+        <is>
+          <t>Bektemir tumani</t>
+        </is>
+      </c>
+      <c r="I155" t="inlineStr">
+        <is>
+          <t>998999290005</t>
+        </is>
+      </c>
+      <c r="J155" t="inlineStr">
+        <is>
+          <t>+998999290005</t>
+        </is>
+      </c>
+      <c r="K155" t="inlineStr">
+        <is>
+          <t>2025-07-02</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="D1:D66"/>
   <mergeCells count="1">

</xml_diff>

<commit_message>
11:02 time 03.07.2025 date
</commit_message>
<xml_diff>
--- a/file_service/qabul.xlsx
+++ b/file_service/qabul.xlsx
@@ -456,7 +456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M155"/>
+  <dimension ref="A1:M157"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
       <selection activeCell="A132" sqref="A132"/>
@@ -9272,6 +9272,120 @@
         </is>
       </c>
     </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>Zafar Jorayev</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>AC2181988</t>
+        </is>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>51708025590020</t>
+        </is>
+      </c>
+      <c r="G156" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H156" t="inlineStr">
+        <is>
+          <t>Yakkasaroy tumani</t>
+        </is>
+      </c>
+      <c r="I156" t="inlineStr">
+        <is>
+          <t>+998930711770</t>
+        </is>
+      </c>
+      <c r="J156" t="inlineStr">
+        <is>
+          <t>+998930711770</t>
+        </is>
+      </c>
+      <c r="K156" t="inlineStr">
+        <is>
+          <t>2025-07-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>Qodirov Abduma'ruf Mahmudovich</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>AD4569027</t>
+        </is>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>50309076530015</t>
+        </is>
+      </c>
+      <c r="G157" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H157" t="inlineStr">
+        <is>
+          <t>Mirobod tumani</t>
+        </is>
+      </c>
+      <c r="I157" t="inlineStr">
+        <is>
+          <t>998991882270</t>
+        </is>
+      </c>
+      <c r="J157" t="inlineStr">
+        <is>
+          <t>+998991882270</t>
+        </is>
+      </c>
+      <c r="K157" t="inlineStr">
+        <is>
+          <t>2025-07-02</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="D1:D66"/>
   <mergeCells count="1">

</xml_diff>

<commit_message>
17:52 time 03.07.2025 date
</commit_message>
<xml_diff>
--- a/file_service/qabul.xlsx
+++ b/file_service/qabul.xlsx
@@ -456,7 +456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M157"/>
+  <dimension ref="A1:M158"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
       <selection activeCell="A132" sqref="A132"/>
@@ -9386,6 +9386,63 @@
         </is>
       </c>
     </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>Zaitova Zulfiya Ruslanovna</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>Psixologiya</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>Rus tili</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>AD5768930</t>
+        </is>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>61001086580034</t>
+        </is>
+      </c>
+      <c r="G158" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H158" t="inlineStr">
+        <is>
+          <t>Bektemir tumani</t>
+        </is>
+      </c>
+      <c r="I158" t="inlineStr">
+        <is>
+          <t>998901155656</t>
+        </is>
+      </c>
+      <c r="J158" t="inlineStr">
+        <is>
+          <t>+998901155656</t>
+        </is>
+      </c>
+      <c r="K158" t="inlineStr">
+        <is>
+          <t>2025-07-03</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="D1:D66"/>
   <mergeCells count="1">

</xml_diff>

<commit_message>
11:04 time 04.07.2025 date
</commit_message>
<xml_diff>
--- a/file_service/qabul.xlsx
+++ b/file_service/qabul.xlsx
@@ -456,7 +456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M158"/>
+  <dimension ref="A1:M159"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
       <selection activeCell="A132" sqref="A132"/>
@@ -9443,6 +9443,63 @@
         </is>
       </c>
     </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>Qaxxarjonov Muhammadkarim Qaxxarjon ogli</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>Bugalteriya hisobi</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>AD2505187</t>
+        </is>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>52801076620023</t>
+        </is>
+      </c>
+      <c r="G159" t="inlineStr">
+        <is>
+          <t>Toshkent viloyati</t>
+        </is>
+      </c>
+      <c r="H159" t="inlineStr">
+        <is>
+          <t>Qibray tumani</t>
+        </is>
+      </c>
+      <c r="I159" t="inlineStr">
+        <is>
+          <t>998777275792</t>
+        </is>
+      </c>
+      <c r="J159" t="inlineStr">
+        <is>
+          <t>+998777275792</t>
+        </is>
+      </c>
+      <c r="K159" t="inlineStr">
+        <is>
+          <t>2025-07-04</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="D1:D66"/>
   <mergeCells count="1">

</xml_diff>

<commit_message>
51:19 time 04.07.2025 date
</commit_message>
<xml_diff>
--- a/file_service/qabul.xlsx
+++ b/file_service/qabul.xlsx
@@ -456,7 +456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M159"/>
+  <dimension ref="A1:M160"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
       <selection activeCell="A132" sqref="A132"/>
@@ -9500,6 +9500,63 @@
         </is>
       </c>
     </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>G'aybullayev Turabek Ulug'bek o'g'li</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>AE1136010</t>
+        </is>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>51008075510046</t>
+        </is>
+      </c>
+      <c r="G160" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H160" t="inlineStr">
+        <is>
+          <t>Shayxontohur tumani</t>
+        </is>
+      </c>
+      <c r="I160" t="inlineStr">
+        <is>
+          <t>998930931308</t>
+        </is>
+      </c>
+      <c r="J160" t="inlineStr">
+        <is>
+          <t>+998930931308</t>
+        </is>
+      </c>
+      <c r="K160" t="inlineStr">
+        <is>
+          <t>2025-07-04</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="D1:D66"/>
   <mergeCells count="1">

</xml_diff>

<commit_message>
18:19 time 12.07.2025 date
</commit_message>
<xml_diff>
--- a/file_service/qabul.xlsx
+++ b/file_service/qabul.xlsx
@@ -456,7 +456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M186"/>
+  <dimension ref="A1:M192"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
       <selection activeCell="A165" sqref="A165:XFD165"/>
@@ -11039,6 +11039,348 @@
         </is>
       </c>
     </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>Baxtiyorov Abdulboriy  Baxrom o'g'li</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>Rus tili</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>AD5552063</t>
+        </is>
+      </c>
+      <c r="F187" t="inlineStr">
+        <is>
+          <t>50612076540028</t>
+        </is>
+      </c>
+      <c r="G187" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H187" t="inlineStr">
+        <is>
+          <t>Shayxontohur tumani</t>
+        </is>
+      </c>
+      <c r="I187" t="inlineStr">
+        <is>
+          <t>998974047888</t>
+        </is>
+      </c>
+      <c r="J187" t="inlineStr">
+        <is>
+          <t>+998950500778</t>
+        </is>
+      </c>
+      <c r="K187" t="inlineStr">
+        <is>
+          <t>2025-07-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>Husanova Nozima Shokir Qizi</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>Inson resurslarini boshqarish</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>AE2838288</t>
+        </is>
+      </c>
+      <c r="F188" t="inlineStr">
+        <is>
+          <t>40409923980013</t>
+        </is>
+      </c>
+      <c r="G188" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="H188" t="inlineStr">
+        <is>
+          <t>Nurobod tumani</t>
+        </is>
+      </c>
+      <c r="I188" t="inlineStr">
+        <is>
+          <t>998938792997</t>
+        </is>
+      </c>
+      <c r="J188" t="inlineStr">
+        <is>
+          <t>+998949381690</t>
+        </is>
+      </c>
+      <c r="K188" t="inlineStr">
+        <is>
+          <t>2025-07-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>Sheralieva Madina Nuralievna</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>Rus tili</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>AE1846105</t>
+        </is>
+      </c>
+      <c r="F189" t="inlineStr">
+        <is>
+          <t>61612078660029</t>
+        </is>
+      </c>
+      <c r="G189" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H189" t="inlineStr">
+        <is>
+          <t>Bektemir tumani</t>
+        </is>
+      </c>
+      <c r="I189" t="inlineStr">
+        <is>
+          <t>998881887967</t>
+        </is>
+      </c>
+      <c r="J189" t="inlineStr">
+        <is>
+          <t>+998970647478</t>
+        </is>
+      </c>
+      <c r="K189" t="inlineStr">
+        <is>
+          <t>2025-07-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>Nurbek Madraimov</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>AD6081351</t>
+        </is>
+      </c>
+      <c r="F190" t="inlineStr">
+        <is>
+          <t>52611076520034</t>
+        </is>
+      </c>
+      <c r="G190" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H190" t="inlineStr">
+        <is>
+          <t>Yashnaobod tumani</t>
+        </is>
+      </c>
+      <c r="I190" t="inlineStr">
+        <is>
+          <t>998974031380</t>
+        </is>
+      </c>
+      <c r="J190" t="inlineStr">
+        <is>
+          <t>+998974031380</t>
+        </is>
+      </c>
+      <c r="K190" t="inlineStr">
+        <is>
+          <t>2025-07-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>Tulyaganov Jafarbek Kozimbek Ogli</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>Ijtimoiy ish</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>AD7166340</t>
+        </is>
+      </c>
+      <c r="F191" t="inlineStr">
+        <is>
+          <t>51404086580054</t>
+        </is>
+      </c>
+      <c r="G191" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H191" t="inlineStr">
+        <is>
+          <t>Yashnaobod tumani</t>
+        </is>
+      </c>
+      <c r="I191" t="inlineStr">
+        <is>
+          <t>998901110800</t>
+        </is>
+      </c>
+      <c r="J191" t="inlineStr">
+        <is>
+          <t>+998901110800</t>
+        </is>
+      </c>
+      <c r="K191" t="inlineStr">
+        <is>
+          <t>2025-07-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>toxtabayeva ruxsora zafar qizi</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>AD4895079</t>
+        </is>
+      </c>
+      <c r="F192" t="inlineStr">
+        <is>
+          <t>60209076790015</t>
+        </is>
+      </c>
+      <c r="G192" t="inlineStr">
+        <is>
+          <t>Toshkent viloyati</t>
+        </is>
+      </c>
+      <c r="H192" t="inlineStr">
+        <is>
+          <t>Piskent tumani</t>
+        </is>
+      </c>
+      <c r="I192" t="inlineStr">
+        <is>
+          <t>998955555207</t>
+        </is>
+      </c>
+      <c r="J192" t="inlineStr">
+        <is>
+          <t>+998955555207</t>
+        </is>
+      </c>
+      <c r="K192" t="inlineStr">
+        <is>
+          <t>2025-07-12</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="D1:D66"/>
   <mergeCells count="1">

</xml_diff>

<commit_message>
11:12 time 14.07.2025 date
</commit_message>
<xml_diff>
--- a/file_service/qabul.xlsx
+++ b/file_service/qabul.xlsx
@@ -456,7 +456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M192"/>
+  <dimension ref="A1:M193"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
       <selection activeCell="A165" sqref="A165:XFD165"/>
@@ -11381,6 +11381,63 @@
         </is>
       </c>
     </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>Jurakulov Alanur Anvarovich</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>AD9626026</t>
+        </is>
+      </c>
+      <c r="F193" t="inlineStr">
+        <is>
+          <t>50112076150040</t>
+        </is>
+      </c>
+      <c r="G193" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="H193" t="inlineStr">
+        <is>
+          <t>Toyloq tumani</t>
+        </is>
+      </c>
+      <c r="I193" t="inlineStr">
+        <is>
+          <t>998948370910</t>
+        </is>
+      </c>
+      <c r="J193" t="inlineStr">
+        <is>
+          <t>+998948370910</t>
+        </is>
+      </c>
+      <c r="K193" t="inlineStr">
+        <is>
+          <t>2025-07-14</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="D1:D66"/>
   <mergeCells count="1">

</xml_diff>

<commit_message>
10:20 time 15.07.2025 date
</commit_message>
<xml_diff>
--- a/file_service/qabul.xlsx
+++ b/file_service/qabul.xlsx
@@ -456,7 +456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M193"/>
+  <dimension ref="A1:M199"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
       <selection activeCell="A165" sqref="A165:XFD165"/>
@@ -11438,6 +11438,348 @@
         </is>
       </c>
     </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>Ibragimova Madina Iskandarovna</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E194" t="inlineStr">
+        <is>
+          <t>AD6450355</t>
+        </is>
+      </c>
+      <c r="F194" t="inlineStr">
+        <is>
+          <t>60706085260040</t>
+        </is>
+      </c>
+      <c r="G194" t="inlineStr">
+        <is>
+          <t>Buxoro viloyati</t>
+        </is>
+      </c>
+      <c r="H194" t="inlineStr">
+        <is>
+          <t>Buxoro tumani</t>
+        </is>
+      </c>
+      <c r="I194" t="inlineStr">
+        <is>
+          <t>998998466696</t>
+        </is>
+      </c>
+      <c r="J194" t="inlineStr">
+        <is>
+          <t>+998770833110</t>
+        </is>
+      </c>
+      <c r="K194" t="inlineStr">
+        <is>
+          <t>2025-07-14</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>Ibragimova Madina Iskandarovna</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E195" t="inlineStr">
+        <is>
+          <t>AD9559203</t>
+        </is>
+      </c>
+      <c r="F195" t="inlineStr">
+        <is>
+          <t>60706085260040</t>
+        </is>
+      </c>
+      <c r="G195" t="inlineStr">
+        <is>
+          <t>Buxoro viloyati</t>
+        </is>
+      </c>
+      <c r="H195" t="inlineStr">
+        <is>
+          <t>Buxoro tumani</t>
+        </is>
+      </c>
+      <c r="I195" t="inlineStr">
+        <is>
+          <t>998998466696</t>
+        </is>
+      </c>
+      <c r="J195" t="inlineStr">
+        <is>
+          <t>+998770833110</t>
+        </is>
+      </c>
+      <c r="K195" t="inlineStr">
+        <is>
+          <t>2025-07-14</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>Sultonov Ogabek</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E196" t="inlineStr">
+        <is>
+          <t>AD8430080</t>
+        </is>
+      </c>
+      <c r="F196" t="inlineStr">
+        <is>
+          <t>51409075540068</t>
+        </is>
+      </c>
+      <c r="G196" t="inlineStr">
+        <is>
+          <t>Jizzax viloyati</t>
+        </is>
+      </c>
+      <c r="H196" t="inlineStr">
+        <is>
+          <t>Jizzax shahri</t>
+        </is>
+      </c>
+      <c r="I196" t="inlineStr">
+        <is>
+          <t>998973250585</t>
+        </is>
+      </c>
+      <c r="J196" t="inlineStr">
+        <is>
+          <t>+998976457717</t>
+        </is>
+      </c>
+      <c r="K196" t="inlineStr">
+        <is>
+          <t>2025-07-14</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>Abduganiyev Asadbek</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>Hayot faoliyati xavfsizligi</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E197" t="inlineStr">
+        <is>
+          <t>AD7448968</t>
+        </is>
+      </c>
+      <c r="F197" t="inlineStr">
+        <is>
+          <t>50212076580022</t>
+        </is>
+      </c>
+      <c r="G197" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H197" t="inlineStr">
+        <is>
+          <t>Yashnaobod tumani</t>
+        </is>
+      </c>
+      <c r="I197" t="inlineStr">
+        <is>
+          <t>998952567674</t>
+        </is>
+      </c>
+      <c r="J197" t="inlineStr">
+        <is>
+          <t>+998952567674</t>
+        </is>
+      </c>
+      <c r="K197" t="inlineStr">
+        <is>
+          <t>2025-07-14</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>Quramboyev Doston</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E198" t="inlineStr">
+        <is>
+          <t>AD1491874</t>
+        </is>
+      </c>
+      <c r="F198" t="inlineStr">
+        <is>
+          <t>50310057110047</t>
+        </is>
+      </c>
+      <c r="G198" t="inlineStr">
+        <is>
+          <t>Xorazm viloyati</t>
+        </is>
+      </c>
+      <c r="H198" t="inlineStr">
+        <is>
+          <t>Gurlan tumani</t>
+        </is>
+      </c>
+      <c r="I198" t="inlineStr">
+        <is>
+          <t>998882032203</t>
+        </is>
+      </c>
+      <c r="J198" t="inlineStr">
+        <is>
+          <t>+998200071691</t>
+        </is>
+      </c>
+      <c r="K198" t="inlineStr">
+        <is>
+          <t>2025-07-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>Hasanov Sherali Nurali o'g'li</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E199" t="inlineStr">
+        <is>
+          <t>AB6269663</t>
+        </is>
+      </c>
+      <c r="F199" t="inlineStr">
+        <is>
+          <t>51411006050012</t>
+        </is>
+      </c>
+      <c r="G199" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="H199" t="inlineStr">
+        <is>
+          <t>Ishtixon tumani</t>
+        </is>
+      </c>
+      <c r="I199" t="inlineStr">
+        <is>
+          <t>998885771060</t>
+        </is>
+      </c>
+      <c r="J199" t="inlineStr">
+        <is>
+          <t>+998885771060</t>
+        </is>
+      </c>
+      <c r="K199" t="inlineStr">
+        <is>
+          <t>2025-07-15</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="D1:D66"/>
   <mergeCells count="1">

</xml_diff>

<commit_message>
14:54 time 15.07.2025 date
</commit_message>
<xml_diff>
--- a/file_service/qabul.xlsx
+++ b/file_service/qabul.xlsx
@@ -456,7 +456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M199"/>
+  <dimension ref="A1:M202"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
       <selection activeCell="A165" sqref="A165:XFD165"/>
@@ -11780,6 +11780,177 @@
         </is>
       </c>
     </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>Nurmatova Rayxon Toxir qizi</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>Mehnat muhofazasi va texnika xavfsizligi</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>Rus tili</t>
+        </is>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E200" t="inlineStr">
+        <is>
+          <t>AD1289454</t>
+        </is>
+      </c>
+      <c r="F200" t="inlineStr">
+        <is>
+          <t>62203066600043</t>
+        </is>
+      </c>
+      <c r="G200" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H200" t="inlineStr">
+        <is>
+          <t>Mirzo Ulugʻbek tumani</t>
+        </is>
+      </c>
+      <c r="I200" t="inlineStr">
+        <is>
+          <t>998947763216</t>
+        </is>
+      </c>
+      <c r="J200" t="inlineStr">
+        <is>
+          <t>+998333906090</t>
+        </is>
+      </c>
+      <c r="K200" t="inlineStr">
+        <is>
+          <t>2025-07-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>Yuldashev Doston Hamza o'g'li</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>Mehnat muhofazasi va texnika xavfsizligi</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>Rus tili</t>
+        </is>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E201" t="inlineStr">
+        <is>
+          <t>AB5180281</t>
+        </is>
+      </c>
+      <c r="F201" t="inlineStr">
+        <is>
+          <t>52509006600014</t>
+        </is>
+      </c>
+      <c r="G201" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H201" t="inlineStr">
+        <is>
+          <t>Mirzo Ulugʻbek tumani</t>
+        </is>
+      </c>
+      <c r="I201" t="inlineStr">
+        <is>
+          <t>998997227826</t>
+        </is>
+      </c>
+      <c r="J201" t="inlineStr">
+        <is>
+          <t>+998976010571</t>
+        </is>
+      </c>
+      <c r="K201" t="inlineStr">
+        <is>
+          <t>2025-07-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>Ziyatov Ahror Ikrom ug'li</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>Psixologiya</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E202" t="inlineStr">
+        <is>
+          <t>AD8979548</t>
+        </is>
+      </c>
+      <c r="F202" t="inlineStr">
+        <is>
+          <t>53006076230033</t>
+        </is>
+      </c>
+      <c r="G202" t="inlineStr">
+        <is>
+          <t>Surxondaryo viloyati</t>
+        </is>
+      </c>
+      <c r="H202" t="inlineStr">
+        <is>
+          <t>Denov tumani</t>
+        </is>
+      </c>
+      <c r="I202" t="inlineStr">
+        <is>
+          <t>998200142003</t>
+        </is>
+      </c>
+      <c r="J202" t="inlineStr">
+        <is>
+          <t>+998200142003</t>
+        </is>
+      </c>
+      <c r="K202" t="inlineStr">
+        <is>
+          <t>2025-07-15</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="D1:D66"/>
   <mergeCells count="1">

</xml_diff>

<commit_message>
11:03 yime 18.07.2025 date
</commit_message>
<xml_diff>
--- a/file_service/qabul.xlsx
+++ b/file_service/qabul.xlsx
@@ -456,7 +456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M202"/>
+  <dimension ref="A1:M224"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
       <selection activeCell="A165" sqref="A165:XFD165"/>
@@ -11951,6 +11951,1260 @@
         </is>
       </c>
     </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>Rasuljonov Fazliddin</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>Bugalteriya hisobi</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E203" t="inlineStr">
+        <is>
+          <t>AD2481404</t>
+        </is>
+      </c>
+      <c r="F203" t="inlineStr">
+        <is>
+          <t>50401076530012</t>
+        </is>
+      </c>
+      <c r="G203" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H203" t="inlineStr">
+        <is>
+          <t>Mirobod tumani</t>
+        </is>
+      </c>
+      <c r="I203" t="inlineStr">
+        <is>
+          <t>998942433422</t>
+        </is>
+      </c>
+      <c r="J203" t="inlineStr">
+        <is>
+          <t>+998942433422</t>
+        </is>
+      </c>
+      <c r="K203" t="inlineStr">
+        <is>
+          <t>2025-07-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>Bazarbayev Samir Quanishbay o'g'li</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E204" t="inlineStr">
+        <is>
+          <t>AD6256423</t>
+        </is>
+      </c>
+      <c r="F204" t="inlineStr">
+        <is>
+          <t>50611077350054</t>
+        </is>
+      </c>
+      <c r="G204" t="inlineStr">
+        <is>
+          <t>Qoraqalpogʻiston Respublikasi</t>
+        </is>
+      </c>
+      <c r="H204" t="inlineStr">
+        <is>
+          <t>Beruniy tumani</t>
+        </is>
+      </c>
+      <c r="I204" t="inlineStr">
+        <is>
+          <t>998997295701</t>
+        </is>
+      </c>
+      <c r="J204" t="inlineStr">
+        <is>
+          <t>+998997295701</t>
+        </is>
+      </c>
+      <c r="K204" t="inlineStr">
+        <is>
+          <t>2025-07-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>Avaznazarov Diyorbek</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E205" t="inlineStr">
+        <is>
+          <t>AD3275498</t>
+        </is>
+      </c>
+      <c r="F205" t="inlineStr">
+        <is>
+          <t>52910065710015</t>
+        </is>
+      </c>
+      <c r="G205" t="inlineStr">
+        <is>
+          <t>Qashqadaryo viloyati</t>
+        </is>
+      </c>
+      <c r="H205" t="inlineStr">
+        <is>
+          <t>Mirishkor tumani</t>
+        </is>
+      </c>
+      <c r="I205" t="inlineStr">
+        <is>
+          <t>998908784346</t>
+        </is>
+      </c>
+      <c r="J205" t="inlineStr">
+        <is>
+          <t>+998950297101</t>
+        </is>
+      </c>
+      <c r="K205" t="inlineStr">
+        <is>
+          <t>2025-07-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>Abdusattorova Shahloxon</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E206" t="inlineStr">
+        <is>
+          <t>AD0332937</t>
+        </is>
+      </c>
+      <c r="F206" t="inlineStr">
+        <is>
+          <t>62808046940058</t>
+        </is>
+      </c>
+      <c r="G206" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="H206" t="inlineStr">
+        <is>
+          <t>Quva tumani</t>
+        </is>
+      </c>
+      <c r="I206" t="inlineStr">
+        <is>
+          <t>998955805054</t>
+        </is>
+      </c>
+      <c r="J206" t="inlineStr">
+        <is>
+          <t>+998916655156</t>
+        </is>
+      </c>
+      <c r="K206" t="inlineStr">
+        <is>
+          <t>2025-07-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>Xasanboyeva Marjona Asatilla qizi</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>Hayot faoliyati xavfsizligi</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E207" t="inlineStr">
+        <is>
+          <t>AD6725608</t>
+        </is>
+      </c>
+      <c r="F207" t="inlineStr">
+        <is>
+          <t>62702086580013</t>
+        </is>
+      </c>
+      <c r="G207" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H207" t="inlineStr">
+        <is>
+          <t>Yashnaobod tumani</t>
+        </is>
+      </c>
+      <c r="I207" t="inlineStr">
+        <is>
+          <t>998993019919</t>
+        </is>
+      </c>
+      <c r="J207" t="inlineStr">
+        <is>
+          <t>+998933519919</t>
+        </is>
+      </c>
+      <c r="K207" t="inlineStr">
+        <is>
+          <t>2025-07-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>Sunnatboyev Asilbek Lutfulloyevich</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>Rus tili</t>
+        </is>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E208" t="inlineStr">
+        <is>
+          <t>AD6172894</t>
+        </is>
+      </c>
+      <c r="F208" t="inlineStr">
+        <is>
+          <t>51102058540026</t>
+        </is>
+      </c>
+      <c r="G208" t="inlineStr">
+        <is>
+          <t>Navoiy viloyati</t>
+        </is>
+      </c>
+      <c r="H208" t="inlineStr">
+        <is>
+          <t>Navoiy shahri</t>
+        </is>
+      </c>
+      <c r="I208" t="inlineStr">
+        <is>
+          <t>998930022274</t>
+        </is>
+      </c>
+      <c r="J208" t="inlineStr">
+        <is>
+          <t>+998931512274</t>
+        </is>
+      </c>
+      <c r="K208" t="inlineStr">
+        <is>
+          <t>2025-07-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>Rahmonov Humoyun Xayitmurodovich</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E209" t="inlineStr">
+        <is>
+          <t>AB2339324</t>
+        </is>
+      </c>
+      <c r="F209" t="inlineStr">
+        <is>
+          <t>30808985700024</t>
+        </is>
+      </c>
+      <c r="G209" t="inlineStr">
+        <is>
+          <t>Qashqadaryo viloyati</t>
+        </is>
+      </c>
+      <c r="H209" t="inlineStr">
+        <is>
+          <t>Kasbi tumani</t>
+        </is>
+      </c>
+      <c r="I209" t="inlineStr">
+        <is>
+          <t>998882090096</t>
+        </is>
+      </c>
+      <c r="J209" t="inlineStr">
+        <is>
+          <t>+998881113261</t>
+        </is>
+      </c>
+      <c r="K209" t="inlineStr">
+        <is>
+          <t>2025-07-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>Sobirjonov Saidjon Obidjon o'g'li</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>Rus tili</t>
+        </is>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E210" t="inlineStr">
+        <is>
+          <t>AC2641623</t>
+        </is>
+      </c>
+      <c r="F210" t="inlineStr">
+        <is>
+          <t>51101045950016</t>
+        </is>
+      </c>
+      <c r="G210" t="inlineStr">
+        <is>
+          <t>Namangan viloyati</t>
+        </is>
+      </c>
+      <c r="H210" t="inlineStr">
+        <is>
+          <t>Yangiqoʻrgʻon tumani</t>
+        </is>
+      </c>
+      <c r="I210" t="inlineStr">
+        <is>
+          <t>998933772113</t>
+        </is>
+      </c>
+      <c r="J210" t="inlineStr">
+        <is>
+          <t>+998772341110</t>
+        </is>
+      </c>
+      <c r="K210" t="inlineStr">
+        <is>
+          <t>2025-07-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>Jasmin Batirova</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E211" t="inlineStr">
+        <is>
+          <t>AD4597593</t>
+        </is>
+      </c>
+      <c r="F211" t="inlineStr">
+        <is>
+          <t>61802077190089</t>
+        </is>
+      </c>
+      <c r="G211" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H211" t="inlineStr">
+        <is>
+          <t>Yunusobod tumani</t>
+        </is>
+      </c>
+      <c r="I211" t="inlineStr">
+        <is>
+          <t>998886872777</t>
+        </is>
+      </c>
+      <c r="J211" t="inlineStr">
+        <is>
+          <t>+998886872777</t>
+        </is>
+      </c>
+      <c r="K211" t="inlineStr">
+        <is>
+          <t>2025-07-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>Maxmadmurodov Karim Orifjon ogli</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>Ijtimoiy ish</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E212" t="inlineStr">
+        <is>
+          <t>AD3677109</t>
+        </is>
+      </c>
+      <c r="F212" t="inlineStr">
+        <is>
+          <t>50203076580028</t>
+        </is>
+      </c>
+      <c r="G212" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H212" t="inlineStr">
+        <is>
+          <t>Yashnaobod tumani</t>
+        </is>
+      </c>
+      <c r="I212" t="inlineStr">
+        <is>
+          <t>998997668641</t>
+        </is>
+      </c>
+      <c r="J212" t="inlineStr">
+        <is>
+          <t>+998997668699</t>
+        </is>
+      </c>
+      <c r="K212" t="inlineStr">
+        <is>
+          <t>2025-07-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>Shohjahon Botirov</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E213" t="inlineStr">
+        <is>
+          <t>AD6006127</t>
+        </is>
+      </c>
+      <c r="F213" t="inlineStr">
+        <is>
+          <t>51107087140013</t>
+        </is>
+      </c>
+      <c r="G213" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H213" t="inlineStr">
+        <is>
+          <t>Yunusobod tumani</t>
+        </is>
+      </c>
+      <c r="I213" t="inlineStr">
+        <is>
+          <t>998950261107</t>
+        </is>
+      </c>
+      <c r="J213" t="inlineStr">
+        <is>
+          <t>+998909451411</t>
+        </is>
+      </c>
+      <c r="K213" t="inlineStr">
+        <is>
+          <t>2025-07-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>Adashboyeva Fotima Qodirali qizi</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E214" t="inlineStr">
+        <is>
+          <t>AD1220503</t>
+        </is>
+      </c>
+      <c r="F214" t="inlineStr">
+        <is>
+          <t>62508005990011</t>
+        </is>
+      </c>
+      <c r="G214" t="inlineStr">
+        <is>
+          <t>Namangan viloyati</t>
+        </is>
+      </c>
+      <c r="H214" t="inlineStr">
+        <is>
+          <t>Mingbuloq tumani</t>
+        </is>
+      </c>
+      <c r="I214" t="inlineStr">
+        <is>
+          <t>79126723290</t>
+        </is>
+      </c>
+      <c r="J214" t="inlineStr">
+        <is>
+          <t>+998333031325</t>
+        </is>
+      </c>
+      <c r="K214" t="inlineStr">
+        <is>
+          <t>2025-07-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>Dilshodova Jasmina Dilshodovna</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>Rus tili</t>
+        </is>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E215" t="inlineStr">
+        <is>
+          <t>AD2836503</t>
+        </is>
+      </c>
+      <c r="F215" t="inlineStr">
+        <is>
+          <t>61709066500066</t>
+        </is>
+      </c>
+      <c r="G215" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H215" t="inlineStr">
+        <is>
+          <t>Uchtepa tumani</t>
+        </is>
+      </c>
+      <c r="I215" t="inlineStr">
+        <is>
+          <t>998773788878</t>
+        </is>
+      </c>
+      <c r="J215" t="inlineStr">
+        <is>
+          <t>+998333704271</t>
+        </is>
+      </c>
+      <c r="K215" t="inlineStr">
+        <is>
+          <t>2025-07-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>Murodova Orzigul Xolmumin qizi</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>Rus tili</t>
+        </is>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E216" t="inlineStr">
+        <is>
+          <t>AD4184431</t>
+        </is>
+      </c>
+      <c r="F216" t="inlineStr">
+        <is>
+          <t>62207076080059</t>
+        </is>
+      </c>
+      <c r="G216" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H216" t="inlineStr">
+        <is>
+          <t>Chilonzor tumani</t>
+        </is>
+      </c>
+      <c r="I216" t="inlineStr">
+        <is>
+          <t>998931312207</t>
+        </is>
+      </c>
+      <c r="J216" t="inlineStr">
+        <is>
+          <t>+998931312207</t>
+        </is>
+      </c>
+      <c r="K216" t="inlineStr">
+        <is>
+          <t>2025-07-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>Shamsiddin Bahodirov Anvar ogli</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E217" t="inlineStr">
+        <is>
+          <t>AD1709792</t>
+        </is>
+      </c>
+      <c r="F217" t="inlineStr">
+        <is>
+          <t>52201056430028</t>
+        </is>
+      </c>
+      <c r="G217" t="inlineStr">
+        <is>
+          <t>Sirdaryo viloyati</t>
+        </is>
+      </c>
+      <c r="H217" t="inlineStr">
+        <is>
+          <t>Mirzaobod tumani</t>
+        </is>
+      </c>
+      <c r="I217" t="inlineStr">
+        <is>
+          <t>998994602082</t>
+        </is>
+      </c>
+      <c r="J217" t="inlineStr">
+        <is>
+          <t>+998990372230</t>
+        </is>
+      </c>
+      <c r="K217" t="inlineStr">
+        <is>
+          <t>2025-07-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>Abdiyev Bunyod</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>AD8597324</t>
+        </is>
+      </c>
+      <c r="F218" t="inlineStr">
+        <is>
+          <t>50604086450020</t>
+        </is>
+      </c>
+      <c r="G218" t="inlineStr">
+        <is>
+          <t>Sirdaryo viloyati</t>
+        </is>
+      </c>
+      <c r="H218" t="inlineStr">
+        <is>
+          <t>Guliston tumani</t>
+        </is>
+      </c>
+      <c r="I218" t="inlineStr">
+        <is>
+          <t>998999090257</t>
+        </is>
+      </c>
+      <c r="J218" t="inlineStr">
+        <is>
+          <t>+998911010257</t>
+        </is>
+      </c>
+      <c r="K218" t="inlineStr">
+        <is>
+          <t>2025-07-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>Xusanboyev Murodbek Sherbek o'g'li</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E219" t="inlineStr">
+        <is>
+          <t>AD9591406</t>
+        </is>
+      </c>
+      <c r="F219" t="inlineStr">
+        <is>
+          <t>52709075530012</t>
+        </is>
+      </c>
+      <c r="G219" t="inlineStr">
+        <is>
+          <t>Jizzax viloyati</t>
+        </is>
+      </c>
+      <c r="H219" t="inlineStr">
+        <is>
+          <t>Yangiobod tumani</t>
+        </is>
+      </c>
+      <c r="I219" t="inlineStr">
+        <is>
+          <t>+998996603300</t>
+        </is>
+      </c>
+      <c r="J219" t="inlineStr">
+        <is>
+          <t>+998995760701</t>
+        </is>
+      </c>
+      <c r="K219" t="inlineStr">
+        <is>
+          <t>2025-07-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>Rasulova Sevinch Kamoliddin qizi</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>AD3631826</t>
+        </is>
+      </c>
+      <c r="F220" t="inlineStr">
+        <is>
+          <t>61206075530012</t>
+        </is>
+      </c>
+      <c r="G220" t="inlineStr">
+        <is>
+          <t>Jizzax viloyati</t>
+        </is>
+      </c>
+      <c r="H220" t="inlineStr">
+        <is>
+          <t>Yangiobod tumani</t>
+        </is>
+      </c>
+      <c r="I220" t="inlineStr">
+        <is>
+          <t>998972011207</t>
+        </is>
+      </c>
+      <c r="J220" t="inlineStr">
+        <is>
+          <t>+998972011207</t>
+        </is>
+      </c>
+      <c r="K220" t="inlineStr">
+        <is>
+          <t>2025-07-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>Murodov Firdavs Ozodbek ogli</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E221" t="inlineStr">
+        <is>
+          <t>AD2765996</t>
+        </is>
+      </c>
+      <c r="F221" t="inlineStr">
+        <is>
+          <t>50907065530015</t>
+        </is>
+      </c>
+      <c r="G221" t="inlineStr">
+        <is>
+          <t>Jizzax viloyati</t>
+        </is>
+      </c>
+      <c r="H221" t="inlineStr">
+        <is>
+          <t>Yangiobod tumani</t>
+        </is>
+      </c>
+      <c r="I221" t="inlineStr">
+        <is>
+          <t>998904020066</t>
+        </is>
+      </c>
+      <c r="J221" t="inlineStr">
+        <is>
+          <t>+998904020066</t>
+        </is>
+      </c>
+      <c r="K221" t="inlineStr">
+        <is>
+          <t>2025-07-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>Botirova Gulmira Quvondiq qizi</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E222" t="inlineStr">
+        <is>
+          <t>AB4552654</t>
+        </is>
+      </c>
+      <c r="F222" t="inlineStr">
+        <is>
+          <t>61702007100017</t>
+        </is>
+      </c>
+      <c r="G222" t="inlineStr">
+        <is>
+          <t>Xorazm viloyati</t>
+        </is>
+      </c>
+      <c r="H222" t="inlineStr">
+        <is>
+          <t>Bogʻot tumani</t>
+        </is>
+      </c>
+      <c r="I222" t="inlineStr">
+        <is>
+          <t>998942331799</t>
+        </is>
+      </c>
+      <c r="J222" t="inlineStr">
+        <is>
+          <t>+998932890124</t>
+        </is>
+      </c>
+      <c r="K222" t="inlineStr">
+        <is>
+          <t>2025-07-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>Amriyeva Nozima</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E223" t="inlineStr">
+        <is>
+          <t>AD8022695</t>
+        </is>
+      </c>
+      <c r="F223" t="inlineStr">
+        <is>
+          <t>61807076110030</t>
+        </is>
+      </c>
+      <c r="G223" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="H223" t="inlineStr">
+        <is>
+          <t>Samarqand shahri</t>
+        </is>
+      </c>
+      <c r="I223" t="inlineStr">
+        <is>
+          <t>998939671807</t>
+        </is>
+      </c>
+      <c r="J223" t="inlineStr">
+        <is>
+          <t>+998939671807</t>
+        </is>
+      </c>
+      <c r="K223" t="inlineStr">
+        <is>
+          <t>2025-07-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>Latipov Akmal Akobirovich</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E224" t="inlineStr">
+        <is>
+          <t>AD0713461</t>
+        </is>
+      </c>
+      <c r="F224" t="inlineStr">
+        <is>
+          <t>32808871110038</t>
+        </is>
+      </c>
+      <c r="G224" t="inlineStr">
+        <is>
+          <t>Buxoro viloyati</t>
+        </is>
+      </c>
+      <c r="H224" t="inlineStr">
+        <is>
+          <t>Jondor tumani</t>
+        </is>
+      </c>
+      <c r="I224" t="inlineStr">
+        <is>
+          <t>+998993103666</t>
+        </is>
+      </c>
+      <c r="J224" t="inlineStr">
+        <is>
+          <t>+998993103666</t>
+        </is>
+      </c>
+      <c r="K224" t="inlineStr">
+        <is>
+          <t>2025-07-18</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="D1:D66"/>
   <mergeCells count="1">

</xml_diff>

<commit_message>
13:11 time 21.07.2025 date
</commit_message>
<xml_diff>
--- a/file_service/qabul.xlsx
+++ b/file_service/qabul.xlsx
@@ -456,7 +456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M224"/>
+  <dimension ref="A1:M232"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
       <selection activeCell="A165" sqref="A165:XFD165"/>
@@ -13205,6 +13205,462 @@
         </is>
       </c>
     </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>Baxtiyorov ulugbek</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>Rus tili</t>
+        </is>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E225" t="inlineStr">
+        <is>
+          <t>AD5227398</t>
+        </is>
+      </c>
+      <c r="F225" t="inlineStr">
+        <is>
+          <t>50811075740064</t>
+        </is>
+      </c>
+      <c r="G225" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H225" t="inlineStr">
+        <is>
+          <t>Yakkasaroy tumani</t>
+        </is>
+      </c>
+      <c r="I225" t="inlineStr">
+        <is>
+          <t>998932407777</t>
+        </is>
+      </c>
+      <c r="J225" t="inlineStr">
+        <is>
+          <t>+998908771777</t>
+        </is>
+      </c>
+      <c r="K225" t="inlineStr">
+        <is>
+          <t>2025-07-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>Ibragimova Zulxumor Atabek Qizi</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E226" t="inlineStr">
+        <is>
+          <t>AD9594019</t>
+        </is>
+      </c>
+      <c r="F226" t="inlineStr">
+        <is>
+          <t>61312067130051</t>
+        </is>
+      </c>
+      <c r="G226" t="inlineStr">
+        <is>
+          <t>Xorazm viloyati</t>
+        </is>
+      </c>
+      <c r="H226" t="inlineStr">
+        <is>
+          <t>Urganch shahri</t>
+        </is>
+      </c>
+      <c r="I226" t="inlineStr">
+        <is>
+          <t>998981118202</t>
+        </is>
+      </c>
+      <c r="J226" t="inlineStr">
+        <is>
+          <t>+998957115151</t>
+        </is>
+      </c>
+      <c r="K226" t="inlineStr">
+        <is>
+          <t>2025-07-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>Ibragimova Dilafruz Atabek qizi</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E227" t="inlineStr">
+        <is>
+          <t>AD9535989</t>
+        </is>
+      </c>
+      <c r="F227" t="inlineStr">
+        <is>
+          <t>60912077130051</t>
+        </is>
+      </c>
+      <c r="G227" t="inlineStr">
+        <is>
+          <t>Xorazm viloyati</t>
+        </is>
+      </c>
+      <c r="H227" t="inlineStr">
+        <is>
+          <t>Urganch tumani</t>
+        </is>
+      </c>
+      <c r="I227" t="inlineStr">
+        <is>
+          <t>998910141284</t>
+        </is>
+      </c>
+      <c r="J227" t="inlineStr">
+        <is>
+          <t>+998946461284</t>
+        </is>
+      </c>
+      <c r="K227" t="inlineStr">
+        <is>
+          <t>2025-07-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>Qosimov Hikmatilla Lutfulla ogli</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E228" t="inlineStr">
+        <is>
+          <t>AD1296541</t>
+        </is>
+      </c>
+      <c r="F228" t="inlineStr">
+        <is>
+          <t>30705910211304</t>
+        </is>
+      </c>
+      <c r="G228" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H228" t="inlineStr">
+        <is>
+          <t>Yashnaobod tumani</t>
+        </is>
+      </c>
+      <c r="I228" t="inlineStr">
+        <is>
+          <t>998974573333</t>
+        </is>
+      </c>
+      <c r="J228" t="inlineStr">
+        <is>
+          <t>+998974573333</t>
+        </is>
+      </c>
+      <c r="K228" t="inlineStr">
+        <is>
+          <t>2025-07-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>Abduxoliqov Iskandarbek Davronjon o'gli</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E229" t="inlineStr">
+        <is>
+          <t>AD4537927</t>
+        </is>
+      </c>
+      <c r="F229" t="inlineStr">
+        <is>
+          <t>52905076920012</t>
+        </is>
+      </c>
+      <c r="G229" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="H229" t="inlineStr">
+        <is>
+          <t>Buvayda tumani</t>
+        </is>
+      </c>
+      <c r="I229" t="inlineStr">
+        <is>
+          <t>998908561835</t>
+        </is>
+      </c>
+      <c r="J229" t="inlineStr">
+        <is>
+          <t>+998975301040</t>
+        </is>
+      </c>
+      <c r="K229" t="inlineStr">
+        <is>
+          <t>2025-07-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>Masharifov masharif murod ogli</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D230" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E230" t="inlineStr">
+        <is>
+          <t>AD4181861</t>
+        </is>
+      </c>
+      <c r="F230" t="inlineStr">
+        <is>
+          <t>51212057130018</t>
+        </is>
+      </c>
+      <c r="G230" t="inlineStr">
+        <is>
+          <t>Xorazm viloyati</t>
+        </is>
+      </c>
+      <c r="H230" t="inlineStr">
+        <is>
+          <t>Urganch tumani</t>
+        </is>
+      </c>
+      <c r="I230" t="inlineStr">
+        <is>
+          <t>998200056838</t>
+        </is>
+      </c>
+      <c r="J230" t="inlineStr">
+        <is>
+          <t>+998918686838</t>
+        </is>
+      </c>
+      <c r="K230" t="inlineStr">
+        <is>
+          <t>2025-07-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>Xoliqov Nuriddin Damirovich</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>Mehnat muhofazasi va texnika xavfsizligi</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D231" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E231" t="inlineStr">
+        <is>
+          <t>AD9119669</t>
+        </is>
+      </c>
+      <c r="F231" t="inlineStr">
+        <is>
+          <t>51710085360046</t>
+        </is>
+      </c>
+      <c r="G231" t="inlineStr">
+        <is>
+          <t>Buxoro viloyati</t>
+        </is>
+      </c>
+      <c r="H231" t="inlineStr">
+        <is>
+          <t>Shofirkon tumani</t>
+        </is>
+      </c>
+      <c r="I231" t="inlineStr">
+        <is>
+          <t>998509008511</t>
+        </is>
+      </c>
+      <c r="J231" t="inlineStr">
+        <is>
+          <t>+998501503580</t>
+        </is>
+      </c>
+      <c r="K231" t="inlineStr">
+        <is>
+          <t>2025-07-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>Hasansher Norboboyev Jaxongir o'g'li</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E232" t="inlineStr">
+        <is>
+          <t>AD0949619</t>
+        </is>
+      </c>
+      <c r="F232" t="inlineStr">
+        <is>
+          <t>50307055680025</t>
+        </is>
+      </c>
+      <c r="G232" t="inlineStr">
+        <is>
+          <t>Qashqadaryo viloyati</t>
+        </is>
+      </c>
+      <c r="H232" t="inlineStr">
+        <is>
+          <t>Kitob tumani</t>
+        </is>
+      </c>
+      <c r="I232" t="inlineStr">
+        <is>
+          <t>998770148278</t>
+        </is>
+      </c>
+      <c r="J232" t="inlineStr">
+        <is>
+          <t>+998770148278</t>
+        </is>
+      </c>
+      <c r="K232" t="inlineStr">
+        <is>
+          <t>2025-07-21</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="D1:D66"/>
   <mergeCells count="1">

</xml_diff>

<commit_message>
11:20 time 22.07.2025 date
</commit_message>
<xml_diff>
--- a/file_service/qabul.xlsx
+++ b/file_service/qabul.xlsx
@@ -456,7 +456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M232"/>
+  <dimension ref="A1:M237"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
       <selection activeCell="A165" sqref="A165:XFD165"/>
@@ -13661,6 +13661,291 @@
         </is>
       </c>
     </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>Ahmadjonov  Doniyorbek Rustamovich</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>Rus tili</t>
+        </is>
+      </c>
+      <c r="D233" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E233" t="inlineStr">
+        <is>
+          <t>AD0562512</t>
+        </is>
+      </c>
+      <c r="F233" t="inlineStr">
+        <is>
+          <t>52107050005111</t>
+        </is>
+      </c>
+      <c r="G233" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="H233" t="inlineStr">
+        <is>
+          <t>Samarqand tumani</t>
+        </is>
+      </c>
+      <c r="I233" t="inlineStr">
+        <is>
+          <t>998992240337</t>
+        </is>
+      </c>
+      <c r="J233" t="inlineStr">
+        <is>
+          <t>+998992240337</t>
+        </is>
+      </c>
+      <c r="K233" t="inlineStr">
+        <is>
+          <t>2025-07-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>Abduraimov Shohjahon Begzodivoch</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E234" t="inlineStr">
+        <is>
+          <t>AE1322337</t>
+        </is>
+      </c>
+      <c r="F234" t="inlineStr">
+        <is>
+          <t>50109085540038</t>
+        </is>
+      </c>
+      <c r="G234" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H234" t="inlineStr">
+        <is>
+          <t>Mirzo Ulugʻbek tumani</t>
+        </is>
+      </c>
+      <c r="I234" t="inlineStr">
+        <is>
+          <t>998911997555</t>
+        </is>
+      </c>
+      <c r="J234" t="inlineStr">
+        <is>
+          <t>+998958127100</t>
+        </is>
+      </c>
+      <c r="K234" t="inlineStr">
+        <is>
+          <t>2025-07-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>Turg'unboyev Shohrux Sardorovich</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>Bugalteriya hisobi</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t>AD6720333</t>
+        </is>
+      </c>
+      <c r="F235" t="inlineStr">
+        <is>
+          <t>52011076830021</t>
+        </is>
+      </c>
+      <c r="G235" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="H235" t="inlineStr">
+        <is>
+          <t>Chilonzor tumani</t>
+        </is>
+      </c>
+      <c r="I235" t="inlineStr">
+        <is>
+          <t>998908270020</t>
+        </is>
+      </c>
+      <c r="J235" t="inlineStr">
+        <is>
+          <t>+998908270020</t>
+        </is>
+      </c>
+      <c r="K235" t="inlineStr">
+        <is>
+          <t>2025-07-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>Abduraxmanov ibroximjon rustamovich</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>Rus tili</t>
+        </is>
+      </c>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E236" t="inlineStr">
+        <is>
+          <t>AD0564279</t>
+        </is>
+      </c>
+      <c r="F236" t="inlineStr">
+        <is>
+          <t>31305795040012</t>
+        </is>
+      </c>
+      <c r="G236" t="inlineStr">
+        <is>
+          <t>Andijon viloyati</t>
+        </is>
+      </c>
+      <c r="H236" t="inlineStr">
+        <is>
+          <t>Andijon tuman</t>
+        </is>
+      </c>
+      <c r="I236" t="inlineStr">
+        <is>
+          <t>998979996656</t>
+        </is>
+      </c>
+      <c r="J236" t="inlineStr">
+        <is>
+          <t>+998502776657</t>
+        </is>
+      </c>
+      <c r="K236" t="inlineStr">
+        <is>
+          <t>2025-07-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>Yulduzova Farida</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>Yurisprudensiya</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>O'zbek tili</t>
+        </is>
+      </c>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>Kunduzgi</t>
+        </is>
+      </c>
+      <c r="E237" t="inlineStr">
+        <is>
+          <t>AD7674668</t>
+        </is>
+      </c>
+      <c r="F237" t="inlineStr">
+        <is>
+          <t>62107075330022</t>
+        </is>
+      </c>
+      <c r="G237" t="inlineStr">
+        <is>
+          <t>Buxoro viloyati</t>
+        </is>
+      </c>
+      <c r="H237" t="inlineStr">
+        <is>
+          <t>Peshku tumani</t>
+        </is>
+      </c>
+      <c r="I237" t="inlineStr">
+        <is>
+          <t>998993842777</t>
+        </is>
+      </c>
+      <c r="J237" t="inlineStr">
+        <is>
+          <t>+998992961425</t>
+        </is>
+      </c>
+      <c r="K237" t="inlineStr">
+        <is>
+          <t>2025-07-22</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="D1:D66"/>
   <mergeCells count="1">

</xml_diff>